<commit_message>
Refactor tests and add atomic db transaction
</commit_message>
<xml_diff>
--- a/clusters/tests/test_models/excel_test_file/Career Landscape Esempio.xlsx
+++ b/clusters/tests/test_models/excel_test_file/Career Landscape Esempio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xpeppers/Desktop/career-landscape/clusters/tests/test_models/excel_test_file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F800CA6B-92B6-8044-93B7-DFC4AD7D92BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47C6BEC-4819-424A-9FB2-5652CC066151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6380" yWindow="3560" windowWidth="25600" windowHeight="14520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Career Landscape" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="39">
   <si>
     <t>Delivery Circle</t>
   </si>
@@ -123,15 +123,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>29-01-2020</t>
-  </si>
-  <si>
-    <t>Cecilia</t>
-  </si>
-  <si>
-    <t>Manzoni</t>
-  </si>
-  <si>
     <t>Delivery</t>
   </si>
   <si>
@@ -151,6 +142,12 @@
   </si>
   <si>
     <t>Recruitment</t>
+  </si>
+  <si>
+    <t>Mario</t>
+  </si>
+  <si>
+    <t>Rossi</t>
   </si>
 </sst>
 </file>
@@ -270,7 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -295,6 +292,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -12487,8 +12485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEBB190-83EC-49FA-B1D1-36A16102E7E2}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12517,18 +12515,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="D2" s="14">
+        <v>43831</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -12552,7 +12550,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="8">
         <v>2</v>
@@ -12588,7 +12586,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="8">
         <v>2</v>
@@ -12631,7 +12629,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -12658,7 +12656,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="8">
         <v>4</v>
@@ -12698,7 +12696,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8">
         <v>3</v>
@@ -12745,7 +12743,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -12770,7 +12768,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8">
         <v>4</v>
@@ -12806,7 +12804,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="8">
         <v>3</v>
@@ -12849,7 +12847,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -12874,7 +12872,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B27" s="8">
         <v>4</v>
@@ -12910,7 +12908,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" s="8">
         <v>3</v>
@@ -12961,7 +12959,7 @@
         <v>21</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>25</v>
@@ -12969,7 +12967,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34" s="8">
         <v>3</v>
@@ -13003,7 +13001,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="8">
         <v>3</v>
@@ -13086,8 +13084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE5355A-31CB-4D53-9CCE-0BBB2BCF55D9}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13116,18 +13114,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="D2" s="14">
+        <v>43831</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -13150,7 +13148,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -13184,7 +13182,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -13218,7 +13216,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -13245,7 +13243,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="8">
         <v>0</v>
@@ -13285,7 +13283,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -13332,7 +13330,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -13357,7 +13355,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8">
         <v>2</v>
@@ -13393,7 +13391,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="8">
         <v>2</v>
@@ -13436,7 +13434,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -13461,7 +13459,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B27" s="8">
         <v>2</v>
@@ -13497,7 +13495,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" s="8">
         <v>3</v>
@@ -13548,7 +13546,7 @@
         <v>21</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>25</v>
@@ -13556,7 +13554,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34" s="8">
         <v>1</v>
@@ -13590,7 +13588,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="8">
         <v>0</v>
@@ -13635,8 +13633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0418BA-1AAD-134E-BE46-D0A37BE2A16A}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13665,18 +13663,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="D2" s="14">
+        <v>43831</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -13699,7 +13697,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B6" s="13">
         <v>0</v>
@@ -13733,7 +13731,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -13767,7 +13765,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -13794,7 +13792,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="8">
         <v>3</v>
@@ -13834,7 +13832,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8">
         <v>0</v>
@@ -13881,7 +13879,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
@@ -13906,7 +13904,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="8">
         <v>1</v>
@@ -13942,7 +13940,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="8">
         <v>0</v>
@@ -13985,7 +13983,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -14010,7 +14008,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B27" s="8">
         <v>3</v>
@@ -14046,7 +14044,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B29" s="8">
         <v>0</v>
@@ -14097,7 +14095,7 @@
         <v>21</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>25</v>
@@ -14105,7 +14103,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B34" s="8">
         <v>4</v>
@@ -14139,7 +14137,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" s="8">
         <v>0</v>

</xml_diff>